<commit_message>
Só no CLIENTE coloquei CLIENTES e coloquei no meio
</commit_message>
<xml_diff>
--- a/Clientes.xlsx
+++ b/Clientes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shirley\Documents\Cursos Engenharia\Digital Pets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gitportalpet\portalpet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,9 +34,6 @@
     <t>Número de Telefone</t>
   </si>
   <si>
-    <t>CLIENTE</t>
-  </si>
-  <si>
     <t>Endereço</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>(31) 3285-5554</t>
+  </si>
+  <si>
+    <t>CLIENTES</t>
   </si>
 </sst>
 </file>
@@ -112,7 +112,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_)@"/>
-    <numFmt numFmtId="166" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+    <numFmt numFmtId="165" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -236,9 +236,6 @@
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -261,7 +258,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -275,6 +272,9 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -304,34 +304,17 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="_)@"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="1" tint="0.24994659260841701"/>
         </left>
         <right/>
         <top/>
         <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="5"/>
-        <name val="Arial"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -367,17 +350,34 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="165" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="5"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="164" formatCode="_)@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="1" tint="0.24994659260841701"/>
         </left>
         <right/>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -541,10 +541,10 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Código do Cliente" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Empresa" dataDxfId="4"/>
-    <tableColumn id="4" name="Endereço" dataDxfId="0"/>
-    <tableColumn id="10" name="Número de Telefone" dataDxfId="1"/>
-    <tableColumn id="12" name="Email" dataDxfId="2"/>
-    <tableColumn id="13" name="Nicho" dataDxfId="3"/>
+    <tableColumn id="4" name="Endereço" dataDxfId="3"/>
+    <tableColumn id="10" name="Número de Telefone" dataDxfId="2"/>
+    <tableColumn id="12" name="Email" dataDxfId="1"/>
+    <tableColumn id="13" name="Nicho" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Customer Contact List" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -783,8 +783,8 @@
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1"/>
@@ -810,8 +810,8 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="36.75" customHeight="1">
-      <c r="B3" s="2" t="s">
-        <v>3</v>
+      <c r="E3" s="17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="7.5" customHeight="1">
@@ -825,293 +825,293 @@
     </row>
     <row r="5" spans="1:8" ht="12" customHeight="1"/>
     <row r="6" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="4" t="s">
+    </row>
+    <row r="7" spans="1:8" ht="17.25" customHeight="1">
+      <c r="A7" s="4"/>
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17.25" customHeight="1">
+      <c r="B8" s="8">
         <v>2</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="C8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17.25" customHeight="1">
+      <c r="B9" s="8">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" customHeight="1">
+      <c r="B10" s="8">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17.25" customHeight="1">
+      <c r="B11" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="17.25" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="9">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B8" s="9">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B9" s="9">
-        <v>3</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B10" s="9">
-        <v>4</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="13" t="s">
+      <c r="C11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B11" s="9">
-        <v>5</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="12" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B12" s="10"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B13" s="10"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B14" s="10"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B15" s="10"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="7"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B16" s="10"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B17" s="10"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B18" s="10"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B19" s="10"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B20" s="10"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B21" s="10"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="7"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B22" s="10"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="7"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B23" s="10"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="7"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B24" s="10"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="7"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="6"/>
     </row>
     <row r="25" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B25" s="10"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="7"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="6"/>
     </row>
     <row r="26" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B26" s="10"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="7"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B27" s="10"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="7"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="6"/>
     </row>
     <row r="28" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B28" s="10"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="7"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B29" s="10"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="7"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B30" s="10"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="7"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="6"/>
     </row>
     <row r="31" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B31" s="10"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="32" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B32" s="10"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="7"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="6"/>
     </row>
     <row r="33" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B33" s="10"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="7"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Alteração e acrescimo de linhas.
</commit_message>
<xml_diff>
--- a/Clientes.xlsx
+++ b/Clientes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gitportalpet\portalpet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB PORTALPET\portalpet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,6 +34,9 @@
     <t>Número de Telefone</t>
   </si>
   <si>
+    <t>CLIENTE</t>
+  </si>
+  <si>
     <t>Endereço</t>
   </si>
   <si>
@@ -101,9 +104,6 @@
   </si>
   <si>
     <t>(31) 3285-5554</t>
-  </si>
-  <si>
-    <t>CLIENTES</t>
   </si>
 </sst>
 </file>
@@ -112,7 +112,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_)@"/>
-    <numFmt numFmtId="165" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+    <numFmt numFmtId="166" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -206,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -223,6 +223,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -236,6 +251,9 @@
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -243,39 +261,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="6" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8" hidden="1" customBuiltin="1"/>
@@ -307,77 +322,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color theme="1" tint="0.24994659260841701"/>
+          <color indexed="64"/>
         </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="5"/>
-        <name val="Arial"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_)@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="5"/>
-        <name val="Arial"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="5"/>
-        <name val="Arial"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_)@"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="1" tint="0.24994659260841701"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -399,13 +360,23 @@
       <numFmt numFmtId="164" formatCode="_)@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color theme="1" tint="0.24994659260841701"/>
+          <color indexed="64"/>
         </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -424,7 +395,144 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_)@"/>
+      <numFmt numFmtId="166" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="5"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="5"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="5"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -784,7 +892,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1"/>
@@ -810,8 +918,8 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="36.75" customHeight="1">
-      <c r="E3" s="17" t="s">
-        <v>26</v>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="7.5" customHeight="1">
@@ -825,293 +933,293 @@
     </row>
     <row r="5" spans="1:8" ht="12" customHeight="1"/>
     <row r="6" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17.25" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17.25" customHeight="1">
+      <c r="B8" s="6">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17.25" customHeight="1">
+      <c r="B9" s="6">
         <v>3</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" customHeight="1">
+      <c r="B10" s="6">
+        <v>4</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17.25" customHeight="1">
+      <c r="B11" s="6">
         <v>5</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="17.25" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B8" s="8">
-        <v>2</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B9" s="8">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B10" s="8">
-        <v>4</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B11" s="8">
-        <v>5</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="12" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B12" s="9"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B13" s="9"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B14" s="9"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B15" s="9"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:8" ht="17.25" customHeight="1">
-      <c r="B16" s="9"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B17" s="9"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B18" s="9"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B19" s="9"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="11"/>
     </row>
     <row r="20" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B20" s="9"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B21" s="9"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B22" s="9"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="11"/>
     </row>
     <row r="23" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B23" s="9"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="11"/>
     </row>
     <row r="24" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B24" s="9"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B25" s="9"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="11"/>
     </row>
     <row r="26" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B26" s="9"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="11"/>
     </row>
     <row r="27" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B27" s="9"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="11"/>
     </row>
     <row r="28" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B28" s="9"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B29" s="9"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B30" s="9"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="11"/>
     </row>
     <row r="31" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B31" s="9"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="11"/>
     </row>
     <row r="32" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B32" s="9"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="11"/>
     </row>
     <row r="33" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B33" s="9"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Lista Sendo Atualizada Online e Offline
</commit_message>
<xml_diff>
--- a/Clientes.xlsx
+++ b/Clientes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes Belo Horizonte Online" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="207">
   <si>
     <t>Código do Cliente</t>
   </si>
@@ -372,6 +372,279 @@
   </si>
   <si>
     <t>Cachorro e Pássaros</t>
+  </si>
+  <si>
+    <t>Clínica Veterinária Marco Antônio</t>
+  </si>
+  <si>
+    <t>R. Itajuba, 654 - Floresta</t>
+  </si>
+  <si>
+    <t>(31) 3423-0128</t>
+  </si>
+  <si>
+    <t>contato@veterinariamarcoantonio.com.br</t>
+  </si>
+  <si>
+    <t>Giselle C. Silva</t>
+  </si>
+  <si>
+    <t>R. Campos Sales, 832 - Gameleira</t>
+  </si>
+  <si>
+    <t>(31) 3371-2598</t>
+  </si>
+  <si>
+    <t>Pet Shop</t>
+  </si>
+  <si>
+    <t>Dog City</t>
+  </si>
+  <si>
+    <t>R. Pedra Bonita, 935 - Barroca</t>
+  </si>
+  <si>
+    <t>(31) 3372-3972</t>
+  </si>
+  <si>
+    <t>contato@dogcityvet.com.br</t>
+  </si>
+  <si>
+    <t>Kollym Pet Shop Boutique</t>
+  </si>
+  <si>
+    <t>Av. Ressaca, 118 Loja 6 - Coração Eucaristico</t>
+  </si>
+  <si>
+    <t>(31) 3412-8704</t>
+  </si>
+  <si>
+    <t>Nikita Pet e Flores</t>
+  </si>
+  <si>
+    <t>R. Coronel Jose Benjamin, 967 - Padre Eustaquio</t>
+  </si>
+  <si>
+    <t>(31) 3464-3016</t>
+  </si>
+  <si>
+    <t>Pet Pampulha</t>
+  </si>
+  <si>
+    <t>Av. Portugal, 2453 - Santa Amelia</t>
+  </si>
+  <si>
+    <t>(31) 3441-7830</t>
+  </si>
+  <si>
+    <t>Bicho Sapeca</t>
+  </si>
+  <si>
+    <t>R. Cuiabá, 186 - Prado</t>
+  </si>
+  <si>
+    <t>(31) 3371-3177</t>
+  </si>
+  <si>
+    <t>Espaço Pet Bh</t>
+  </si>
+  <si>
+    <t>Av. José Cândido da Silveira, 571 - Cidade Nova</t>
+  </si>
+  <si>
+    <t>(31) 2512-0011</t>
+  </si>
+  <si>
+    <t>Dog Clean</t>
+  </si>
+  <si>
+    <t>R. S. Gonçalo, 976 - Das Graças</t>
+  </si>
+  <si>
+    <t>Bichos da Serra</t>
+  </si>
+  <si>
+    <t>R. do Ouro, 272 - Serra</t>
+  </si>
+  <si>
+    <t>(31) 3264-9876</t>
+  </si>
+  <si>
+    <t>Bernis e Melo Com. de Ração e Pet shop</t>
+  </si>
+  <si>
+    <t>Pet It Shop</t>
+  </si>
+  <si>
+    <t>Av. Carandaí, 178 Loja 1 - Funcionários</t>
+  </si>
+  <si>
+    <t>(31) 3024-0434</t>
+  </si>
+  <si>
+    <t>Cão Bom Pet Shop</t>
+  </si>
+  <si>
+    <t>R. Porto Seguro, 589 - Nova Vista</t>
+  </si>
+  <si>
+    <t>(31) 3485-8386</t>
+  </si>
+  <si>
+    <t>Lat &amp; Mia</t>
+  </si>
+  <si>
+    <t>R. Serro, 315 - Bonfim</t>
+  </si>
+  <si>
+    <t>(31) 3422-4692</t>
+  </si>
+  <si>
+    <t>Banho e Tosa Cão Bonito</t>
+  </si>
+  <si>
+    <t>R. Araguari, 1370 - Barro Preto</t>
+  </si>
+  <si>
+    <t>(31) 9171-1289</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bicho Fino </t>
+  </si>
+  <si>
+    <t>R. Desembargador Cintra Neto, 420 - Milionários</t>
+  </si>
+  <si>
+    <t>(31) 3321-8086</t>
+  </si>
+  <si>
+    <t>Rei do Cachorro</t>
+  </si>
+  <si>
+    <t>Av. Augusto de Lima, 744 - Centro</t>
+  </si>
+  <si>
+    <t>(31) 8735-3012</t>
+  </si>
+  <si>
+    <t>Pet Shop Doçura</t>
+  </si>
+  <si>
+    <t>R. Dr. Plinio Moraes, 468 - Cidade Nova</t>
+  </si>
+  <si>
+    <t>(31) 3484-6880</t>
+  </si>
+  <si>
+    <t>Pop Dog</t>
+  </si>
+  <si>
+    <t>R. Salinas,1815 - Floresta</t>
+  </si>
+  <si>
+    <t>(31) 2555-2197</t>
+  </si>
+  <si>
+    <t>Atelier do Cão</t>
+  </si>
+  <si>
+    <t>R. Santa Catarina, 1141 - Floresta</t>
+  </si>
+  <si>
+    <t>(31) 3337-9467</t>
+  </si>
+  <si>
+    <t>Mania de Cão</t>
+  </si>
+  <si>
+    <t>R. dos Timbiras, 2250 Sala 101 - Santo Agostinho</t>
+  </si>
+  <si>
+    <t>(31) 3292-3592</t>
+  </si>
+  <si>
+    <t>Mundo dos Bichos</t>
+  </si>
+  <si>
+    <t>R. Bernardo Guimarães, 1873  - Lourdes</t>
+  </si>
+  <si>
+    <t>(31) 3291-1605</t>
+  </si>
+  <si>
+    <t>Pet Hotel &amp; Day Care Pet Creche</t>
+  </si>
+  <si>
+    <t>R. Marilio Gomes Silveira, 1014 - Milionários</t>
+  </si>
+  <si>
+    <t>(31) 3234-5991</t>
+  </si>
+  <si>
+    <t>Cantinho dos Animais</t>
+  </si>
+  <si>
+    <t>R. Santa Catarina, 201 Loja 601 - Centro</t>
+  </si>
+  <si>
+    <t>(31) 3274-9397</t>
+  </si>
+  <si>
+    <t>Mascote Veterinária</t>
+  </si>
+  <si>
+    <t>R. Professor Pimenta Veiga, 531 - Cidade Nova</t>
+  </si>
+  <si>
+    <t>(31) 3484-1211</t>
+  </si>
+  <si>
+    <t>Veterinário</t>
+  </si>
+  <si>
+    <t>O Ponto da Ração</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Av. Edgard Torres, 720 - Minas Caixa </t>
+  </si>
+  <si>
+    <t>(31) 3455-6892</t>
+  </si>
+  <si>
+    <t>Meu Amigo Fiel</t>
+  </si>
+  <si>
+    <t>Av. Augusto dos Anjos, 208 - Santa Mônica</t>
+  </si>
+  <si>
+    <t>(31) 3452-7450</t>
+  </si>
+  <si>
+    <t>Sagradog</t>
+  </si>
+  <si>
+    <t>R. João Gualberto Filho, 196 Loja 10 - Sagrada Família</t>
+  </si>
+  <si>
+    <t>(31) 3463-9787</t>
+  </si>
+  <si>
+    <t>Exotic Pet Show</t>
+  </si>
+  <si>
+    <t>R. S. Joaquim, 516 - Sagrada Família</t>
+  </si>
+  <si>
+    <t>(31) 2531-1598</t>
+  </si>
+  <si>
+    <t>Dog House</t>
+  </si>
+  <si>
+    <t>R. Euclasio, 669 - Paraiso</t>
+  </si>
+  <si>
+    <t>(31) 3283-2365</t>
   </si>
 </sst>
 </file>
@@ -1401,8 +1674,8 @@
   </sheetPr>
   <dimension ref="A1:G156"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1411,7 +1684,7 @@
     <col min="2" max="2" width="30.42578125" customWidth="1"/>
     <col min="3" max="3" width="58.42578125" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" customWidth="1"/>
     <col min="6" max="6" width="51.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
   </cols>
@@ -1686,7 +1959,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>13</v>
       </c>
@@ -1706,7 +1979,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>14</v>
       </c>
@@ -2063,20 +2336,44 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="10"/>
+      <c r="A38" s="6">
+        <v>33</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="10"/>
+      <c r="A39" s="6">
+        <v>34</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
@@ -2287,14 +2584,16 @@
     <hyperlink ref="E26" r:id="rId11"/>
     <hyperlink ref="E33" r:id="rId12"/>
     <hyperlink ref="E34" r:id="rId13"/>
+    <hyperlink ref="E38" r:id="rId14"/>
+    <hyperlink ref="E39" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="50" fitToHeight="0" orientation="landscape" r:id="rId14"/>
+  <pageSetup paperSize="9" scale="50" fitToHeight="0" orientation="landscape" r:id="rId16"/>
   <headerFooter differentFirst="1">
     <oddFooter>Página &amp;P de &amp;N</oddFooter>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2303,14 +2602,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F50"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
     <col min="3" max="3" width="58.42578125" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="37.28515625" customWidth="1"/>
@@ -2359,228 +2658,508 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>122</v>
+      </c>
       <c r="E6" s="11"/>
-      <c r="F6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>130</v>
+      </c>
       <c r="E7" s="11"/>
-      <c r="F7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
+      <c r="A8" s="6">
+        <v>3</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>133</v>
+      </c>
       <c r="E8" s="12"/>
-      <c r="F8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
+      <c r="A9" s="6">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="E9" s="13"/>
-      <c r="F9" s="10"/>
+      <c r="F9" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
+      <c r="A10" s="6">
+        <v>5</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>139</v>
+      </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="10"/>
+      <c r="F10" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
+      <c r="A11" s="6">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="E11" s="13"/>
-      <c r="F11" s="10"/>
+      <c r="F11" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="9"/>
+      <c r="A12" s="6">
+        <v>7</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="E12" s="13"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
+      <c r="A13" s="6">
+        <v>8</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>147</v>
+      </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="10"/>
+      <c r="F13" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
+      <c r="A14" s="6">
+        <v>9</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="E14" s="11"/>
-      <c r="F14" s="10"/>
+      <c r="F14" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
+      <c r="A15" s="6">
+        <v>10</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>151</v>
+      </c>
       <c r="E15" s="11"/>
-      <c r="F15" s="10"/>
+      <c r="F15" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
+      <c r="A16" s="6">
+        <v>11</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>154</v>
+      </c>
       <c r="E16" s="11"/>
-      <c r="F16" s="10"/>
+      <c r="F16" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
+      <c r="A17" s="6">
+        <v>12</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>157</v>
+      </c>
       <c r="E17" s="11"/>
-      <c r="F17" s="10"/>
+      <c r="F17" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
+      <c r="A18" s="6">
+        <v>13</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>160</v>
+      </c>
       <c r="E18" s="11"/>
-      <c r="F18" s="10"/>
+      <c r="F18" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
+      <c r="A19" s="6">
+        <v>14</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>163</v>
+      </c>
       <c r="E19" s="13"/>
-      <c r="F19" s="10"/>
+      <c r="F19" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
+      <c r="A20" s="6">
+        <v>15</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>166</v>
+      </c>
       <c r="E20" s="13"/>
-      <c r="F20" s="10"/>
+      <c r="F20" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
+      <c r="A21" s="6">
+        <v>16</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>169</v>
+      </c>
       <c r="E21" s="13"/>
-      <c r="F21" s="10"/>
+      <c r="F21" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
+      <c r="A22" s="6">
+        <v>17</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>172</v>
+      </c>
       <c r="E22" s="11"/>
-      <c r="F22" s="10"/>
+      <c r="F22" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
+      <c r="A23" s="6">
+        <v>18</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>175</v>
+      </c>
       <c r="E23" s="11"/>
-      <c r="F23" s="10"/>
+      <c r="F23" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
+      <c r="A24" s="6">
+        <v>19</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>178</v>
+      </c>
       <c r="E24" s="11"/>
-      <c r="F24" s="10"/>
+      <c r="F24" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
+      <c r="A25" s="6">
+        <v>20</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>181</v>
+      </c>
       <c r="E25" s="11"/>
-      <c r="F25" s="10"/>
+      <c r="F25" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
+      <c r="A26" s="6">
+        <v>21</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>184</v>
+      </c>
       <c r="E26" s="11"/>
-      <c r="F26" s="10"/>
+      <c r="F26" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
+      <c r="A27" s="6">
+        <v>22</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>187</v>
+      </c>
       <c r="E27" s="13"/>
-      <c r="F27" s="10"/>
+      <c r="F27" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
+      <c r="A28" s="6">
+        <v>23</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>190</v>
+      </c>
       <c r="E28" s="13"/>
-      <c r="F28" s="10"/>
+      <c r="F28" s="10" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
+      <c r="A29" s="6">
+        <v>24</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>194</v>
+      </c>
       <c r="E29" s="13"/>
-      <c r="F29" s="10"/>
+      <c r="F29" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
+      <c r="A30" s="6">
+        <v>25</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>197</v>
+      </c>
       <c r="E30" s="13"/>
-      <c r="F30" s="10"/>
+      <c r="F30" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
+      <c r="A31" s="6">
+        <v>26</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>200</v>
+      </c>
       <c r="E31" s="13"/>
-      <c r="F31" s="10"/>
+      <c r="F31" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
+      <c r="A32" s="6">
+        <v>27</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="E32" s="13"/>
-      <c r="F32" s="10"/>
+      <c r="F32" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
+      <c r="A33" s="6">
+        <v>28</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>206</v>
+      </c>
       <c r="E33" s="14"/>
-      <c r="F33" s="10"/>
+      <c r="F33" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>

</xml_diff>